<commit_message>
try something new in fsl_cleaning and add iycf_flags
</commit_message>
<xml_diff>
--- a/inst/iycf_quality_report/resources/flag_description.xlsx
+++ b/inst/iycf_quality_report/resources/flag_description.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\IPHRA_toolkit\cleaning\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\iycf_quality_report\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{688B33F7-C545-4314-91D9-91FBB54A4148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29649B2-1D1E-4A22-9906-42AF071E1353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FSL" sheetId="1" r:id="rId1"/>
     <sheet name="WASH" sheetId="2" r:id="rId2"/>
     <sheet name="NUT" sheetId="3" r:id="rId3"/>
     <sheet name="MORT" sheetId="4" r:id="rId4"/>
+    <sheet name="IYCF" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="171">
   <si>
     <t>flag_name</t>
   </si>
@@ -458,6 +459,90 @@
   </si>
   <si>
     <t>Respondent reported sex of dead person male and a cause of death related to female only.</t>
+  </si>
+  <si>
+    <t> flag_name</t>
+  </si>
+  <si>
+    <t>flag_yes_foods</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming all foods groups</t>
+  </si>
+  <si>
+    <t>Review with enumerators since its unlikely and implausible that the child consumed ALL the food groups</t>
+  </si>
+  <si>
+    <t>flag_yes_liquids</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming all liquids groups</t>
+  </si>
+  <si>
+    <t>Review with enumerators since its unlikely and implausible that the child consumed ALL the liquid groups</t>
+  </si>
+  <si>
+    <t>flag_no_anything</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming no foods or liquids groups at all</t>
+  </si>
+  <si>
+    <t>Check child age if &lt;9 months and IF exclusively breastfeeding. If child is not exclusively breastfeeding and &gt;9 months, then review with enumerator as its extremely unlikely that child did not consume any foods or liquids.</t>
+  </si>
+  <si>
+    <t>flag_no_foods</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming no foods groups while reporting eating solid or semi-solid food meals</t>
+  </si>
+  <si>
+    <t>Review with enumerators since its erroneous that the child was reported to consume NO food groups YET ate solid or semi-solid food meals</t>
+  </si>
+  <si>
+    <t>flag_all_foods_no_meal</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming all foods groups while reporting not eating any solid or semi-solid food meals</t>
+  </si>
+  <si>
+    <t>Review with enumerators since its erroneous that the child was reported to consume ALL 8 food groups YET did not eat any solid or semi-solid food meals</t>
+  </si>
+  <si>
+    <t>flag_some_foods_no_meal</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming some foods groups while reporting not eating any solid or semi-solid food meals</t>
+  </si>
+  <si>
+    <t>Review with enumerators since its erroneous that the child was reported to consume SOME food groups YET did not eat any solid or semi-solid food meals</t>
+  </si>
+  <si>
+    <t>flag_high_mdd_low_mmf</t>
+  </si>
+  <si>
+    <t>Respondent reported high mdd score while reporting low meal frequency consumed (&lt;=1)</t>
+  </si>
+  <si>
+    <t>If MDD is high (&gt;4) and meal frequency is low (&lt;=1), review for enumerator bias/error</t>
+  </si>
+  <si>
+    <t>flag_under6_nobf_nomilk</t>
+  </si>
+  <si>
+    <t>Respondent reported child under 6 month and not breastfed and no milk given</t>
+  </si>
+  <si>
+    <t>If child is &lt;6months AND not breastfed AND no other milks given, review for enumerator bias/error</t>
+  </si>
+  <si>
+    <t>flag_meats_nostaples</t>
+  </si>
+  <si>
+    <t>Respondent reported child consuming meats but no staples</t>
+  </si>
+  <si>
+    <t>Review with enumerators since its unlikely and implausible that the child consumed meats but NO staples.</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8440C440-E586-4116-9669-C7C58F9A3DB2}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -1455,4 +1540,133 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3A0A52-B0A2-4FB2-82DB-E5507B17F377}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>168</v>
+      </c>
+      <c r="B10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add iycf cleaning and update couple of minor fixes
</commit_message>
<xml_diff>
--- a/inst/iycf_quality_report/resources/flag_description.xlsx
+++ b/inst/iycf_quality_report/resources/flag_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abraham.azar\Desktop\git\impactR4PHU\inst\iycf_quality_report\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8A5FCB-6E38-4A77-8F2F-6B88E93F876C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6054A58F-1C05-4B62-B71D-23CE185E0B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1544,13 +1544,13 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="2" max="2" width="109.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>